<commit_message>
Rental - API Cliente e Veiculo
</commit_message>
<xml_diff>
--- a/Exercícios/01_rental/Modelagem/Exercicio1.2-Locadora-FÍSICO.xlsx
+++ b/Exercícios/01_rental/Modelagem/Exercicio1.2-Locadora-FÍSICO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/480d5ffb018c6fc9/Documentos/SENAI/2DM_Backend_API/Exercícios/01_rental/Modelagem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="316" documentId="11_AD4D361C20488DEA4E38A0CD341D69CE5ADEDD9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B98256FD-6C45-4C53-A5DC-3892A417D77B}"/>
+  <xr:revisionPtr revIDLastSave="369" documentId="11_AD4D361C20488DEA4E38A0CD341D69CE5ADEDD9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE364C7D-BF96-42E5-A997-B3BB1E574D08}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10350" yWindow="2310" windowWidth="10140" windowHeight="7020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -157,7 +157,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +203,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -442,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -496,9 +504,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -571,6 +576,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +883,7 @@
     <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -882,10 +894,10 @@
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -898,6 +910,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="5"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
@@ -905,103 +918,103 @@
         <v>1</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>4</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="Q2" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="59">
-        <v>1</v>
-      </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="61" t="s">
+      <c r="A3" s="58">
+        <v>1</v>
+      </c>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="60"/>
+      <c r="D3" s="59"/>
       <c r="F3" s="16">
         <v>1</v>
       </c>
       <c r="G3" s="11">
         <v>1</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="8">
+        <v>4</v>
+      </c>
+      <c r="I3" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="32">
-        <v>11</v>
-      </c>
-      <c r="K3" s="23">
-        <v>4</v>
-      </c>
-      <c r="L3" s="26" t="s">
+      <c r="K3" s="31">
+        <v>1</v>
+      </c>
+      <c r="L3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="28">
+      <c r="M3" s="9">
+        <v>3</v>
+      </c>
+      <c r="N3" s="27">
         <v>2019</v>
       </c>
-      <c r="O3" s="8">
-        <v>6</v>
-      </c>
-      <c r="P3" s="33">
+      <c r="P3" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="26" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
       <c r="F4" s="19">
         <v>2</v>
       </c>
       <c r="G4" s="11">
         <v>1</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="9">
+        <v>5</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="33">
-        <v>22</v>
-      </c>
-      <c r="K4" s="20">
-        <v>3</v>
-      </c>
-      <c r="L4" s="27" t="s">
+      <c r="K4" s="32">
+        <v>2</v>
+      </c>
+      <c r="L4" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="29">
+      <c r="M4" s="9">
+        <v>1</v>
+      </c>
+      <c r="N4" s="28">
         <v>2017</v>
       </c>
-      <c r="O4" s="9">
-        <v>7</v>
-      </c>
-      <c r="P4" s="35">
-        <v>44</v>
-      </c>
-      <c r="Q4" s="27" t="s">
+      <c r="P4" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="26" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1012,28 +1025,28 @@
       <c r="G5" s="11">
         <v>1</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="9">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="34">
-        <v>33</v>
-      </c>
-      <c r="K5" s="24">
-        <v>5</v>
-      </c>
-      <c r="L5" s="27" t="s">
+      <c r="K5" s="33">
+        <v>3</v>
+      </c>
+      <c r="L5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="29">
+      <c r="M5" s="9">
+        <v>4</v>
+      </c>
+      <c r="N5" s="28">
         <v>2015</v>
       </c>
-      <c r="O5" s="9">
-        <v>8</v>
-      </c>
-      <c r="P5" s="32">
-        <v>11</v>
-      </c>
-      <c r="Q5" s="27" t="s">
+      <c r="P5" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="26" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1044,28 +1057,28 @@
       <c r="G6" s="11">
         <v>1</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="35">
-        <v>44</v>
-      </c>
-      <c r="K6" s="18">
-        <v>1</v>
-      </c>
-      <c r="L6" s="27" t="s">
+      <c r="K6" s="34">
+        <v>4</v>
+      </c>
+      <c r="L6" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="29">
+      <c r="M6" s="9">
+        <v>2</v>
+      </c>
+      <c r="N6" s="28">
         <v>2016</v>
       </c>
-      <c r="O6" s="9">
-        <v>9</v>
-      </c>
-      <c r="P6" s="34">
-        <v>33</v>
-      </c>
-      <c r="Q6" s="27" t="s">
+      <c r="P6" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="26" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1076,26 +1089,26 @@
       <c r="G7" s="14">
         <v>1</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="10">
+        <v>3</v>
+      </c>
+      <c r="I7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="36">
-        <v>55</v>
-      </c>
-      <c r="K7" s="25">
-        <v>2</v>
+      <c r="K7" s="35">
+        <v>5</v>
       </c>
       <c r="L7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="30">
+      <c r="M7" s="10">
+        <v>5</v>
+      </c>
+      <c r="N7" s="29">
         <v>2020</v>
       </c>
-      <c r="O7" s="10">
-        <v>0</v>
-      </c>
-      <c r="P7" s="36">
-        <v>55</v>
+      <c r="P7" s="10">
+        <v>5</v>
       </c>
       <c r="Q7" s="13" t="s">
         <v>27</v>
@@ -1108,9 +1121,9 @@
       <c r="G10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1138,15 +1151,15 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="40">
-        <v>1</v>
-      </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42" t="s">
+      <c r="A12" s="39">
+        <v>1</v>
+      </c>
+      <c r="B12" s="40"/>
+      <c r="C12" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="55" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="54" t="s">
         <v>38</v>
       </c>
       <c r="G12" s="17">
@@ -1155,48 +1168,48 @@
       <c r="H12" s="20">
         <v>3</v>
       </c>
-      <c r="I12" s="49">
+      <c r="I12" s="48">
         <v>2</v>
       </c>
-      <c r="J12" s="53">
+      <c r="J12" s="52">
         <v>44242</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="43">
+      <c r="A13" s="42">
         <v>2</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="45" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="56" t="s">
+      <c r="D13" s="38"/>
+      <c r="E13" s="55" t="s">
         <v>39</v>
       </c>
       <c r="G13" s="17">
         <v>222</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="23">
         <v>5</v>
       </c>
-      <c r="I13" s="50">
+      <c r="I13" s="49">
         <v>3</v>
       </c>
-      <c r="J13" s="53">
+      <c r="J13" s="52">
         <v>44346</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="46">
+      <c r="A14" s="45">
         <v>3</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48" t="s">
+      <c r="B14" s="46"/>
+      <c r="C14" s="47" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="56" t="s">
         <v>40</v>
       </c>
       <c r="G14" s="9">
@@ -1205,24 +1218,24 @@
       <c r="H14" s="18">
         <v>1</v>
       </c>
-      <c r="I14" s="51">
-        <v>1</v>
-      </c>
-      <c r="J14" s="53">
+      <c r="I14" s="50">
+        <v>1</v>
+      </c>
+      <c r="J14" s="52">
         <v>44400</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G15" s="31">
+      <c r="G15" s="30">
         <v>444</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="24">
         <v>2</v>
       </c>
-      <c r="I15" s="52">
+      <c r="I15" s="51">
         <v>2</v>
       </c>
-      <c r="J15" s="54">
+      <c r="J15" s="53">
         <v>44410</v>
       </c>
     </row>

</xml_diff>